<commit_message>
this my second commit
</commit_message>
<xml_diff>
--- a/TestData/creatpagexlfile.xlsx
+++ b/TestData/creatpagexlfile.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>locator</t>
   </si>
@@ -112,13 +112,28 @@
   </si>
   <si>
     <t>1995</t>
+  </si>
+  <si>
+    <t>test_login data</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>mech712712114023</t>
+  </si>
+  <si>
+    <t>login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,13 +149,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -156,7 +184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -166,6 +194,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -468,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,14 +688,66 @@
         <v>5</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A13:E13"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1"/>
     <hyperlink ref="D6" r:id="rId2"/>
     <hyperlink ref="D7" r:id="rId3"/>
+    <hyperlink ref="D14" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>